<commit_message>
Finish final program for the contest
</commit_message>
<xml_diff>
--- a/Face_recognition/Users/Joshua.xlsx
+++ b/Face_recognition/Users/Joshua.xlsx
@@ -382,7 +382,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.031557985</v>
+        <v>-0.108838172</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -390,7 +390,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.07195568099999999</v>
+        <v>0.102213206</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.018875856</v>
+        <v>0.035056553</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -406,7 +406,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.029561868</v>
+        <v>-0.07317942199999999</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -414,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.027486166</v>
+        <v>-0.075632767</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -422,7 +422,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.045763325</v>
+        <v>-0.048480942</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -430,7 +430,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.016208712</v>
+        <v>-0.026082961</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.083266124</v>
+        <v>-0.104705686</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -446,7 +446,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.173702478</v>
+        <v>0.133157355</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -454,7 +454,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.120406784</v>
+        <v>-0.082395143</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.28800866</v>
+        <v>0.268702188</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -470,7 +470,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.055995867</v>
+        <v>-0.048298507</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -478,7 +478,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.218066305</v>
+        <v>-0.192681301</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -486,7 +486,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.116420642</v>
+        <v>-0.152074051</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -494,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.015650094</v>
+        <v>-0.052721073</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -502,7 +502,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.17619364</v>
+        <v>0.183200194</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -510,7 +510,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-0.172071084</v>
+        <v>-0.18698998</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -518,7 +518,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-0.12494386</v>
+        <v>-0.138461451</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -526,7 +526,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.044352341</v>
+        <v>-0.00775468</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -534,7 +534,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.007630357</v>
+        <v>-0.010484921</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -542,7 +542,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.09166386</v>
+        <v>0.124480542</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -550,7 +550,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.024387656</v>
+        <v>-0.020797776</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -558,7 +558,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-0.004870723</v>
+        <v>-0.009224501</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -566,7 +566,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.003710908</v>
+        <v>0.043361183</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -574,7 +574,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.000390306</v>
+        <v>-0.076622804</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -582,7 +582,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-0.339600265</v>
+        <v>-0.32262107</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -590,7 +590,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-0.130785137</v>
+        <v>-0.09768600199999999</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -598,7 +598,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-0.03998651</v>
+        <v>-0.079447407</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -606,7 +606,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.039208911</v>
+        <v>0.027373529</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -614,7 +614,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>-0.059106097</v>
+        <v>-0.079167162</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -622,7 +622,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-0.025551479</v>
+        <v>-0.023174303</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -630,7 +630,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.06424898699999999</v>
+        <v>0.037933061</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -638,7 +638,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-0.159567058</v>
+        <v>-0.183819699</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -646,7 +646,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>-0.102386832</v>
+        <v>-0.07962683500000001</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -654,7 +654,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.055909052</v>
+        <v>-0.006608619</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -662,7 +662,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.045633197</v>
+        <v>0.076644039</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -670,7 +670,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>-0.026887234</v>
+        <v>-0.002825303</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -678,7 +678,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>-0.046689477</v>
+        <v>-0.048441424</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -686,7 +686,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.198813468</v>
+        <v>0.126694449</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -694,7 +694,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>-0.025923625</v>
+        <v>-0.026727514</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -702,7 +702,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>-0.210282162</v>
+        <v>-0.20244848</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -710,7 +710,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.013121577</v>
+        <v>0.038890875</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -718,7 +718,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.11662896</v>
+        <v>0.038352084</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -726,7 +726,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.251678079</v>
+        <v>0.239657096</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -734,7 +734,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.147043929</v>
+        <v>0.190517519</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -742,7 +742,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.061370287</v>
+        <v>0.041690889</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -750,7 +750,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>-0.006444454</v>
+        <v>0.033719902</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -758,7 +758,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>-0.159316421</v>
+        <v>-0.188193707</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -766,7 +766,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.07675623099999999</v>
+        <v>0.096049495</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -774,7 +774,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>-0.09507899</v>
+        <v>-0.141508164</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -782,7 +782,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.036550421</v>
+        <v>0.032553968</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -790,7 +790,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.125107616</v>
+        <v>0.130092783</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -798,7 +798,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.167219177</v>
+        <v>0.061158116</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -806,7 +806,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.07188544400000001</v>
+        <v>0.056411231</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -814,7 +814,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.022034686</v>
+        <v>-0.02537516</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -822,7 +822,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>-0.121873207</v>
+        <v>-0.119164277</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -830,7 +830,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.036276888</v>
+        <v>0.02497834</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -838,7 +838,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.123752311</v>
+        <v>0.08360324199999999</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -846,7 +846,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>-0.188704565</v>
+        <v>-0.147494283</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -854,7 +854,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.035658937</v>
+        <v>0.007501006</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -862,7 +862,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.084504157</v>
+        <v>0.079947359</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -870,7 +870,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>-0.105487689</v>
+        <v>-0.07790449000000001</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -878,7 +878,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>-0.0208176</v>
+        <v>-0.050433668</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -886,7 +886,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>-0.051254872</v>
+        <v>-0.115189413</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -894,7 +894,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.228359595</v>
+        <v>0.222678571</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -902,7 +902,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-0.001519723</v>
+        <v>0.054921989</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -910,7 +910,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>-0.113097988</v>
+        <v>-0.119217342</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -918,7 +918,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>-0.228689149</v>
+        <v>-0.202754533</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -926,7 +926,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.101438843</v>
+        <v>0.142159313</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -934,7 +934,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>-0.151493579</v>
+        <v>-0.135585723</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -942,7 +942,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>-0.092212081</v>
+        <v>-0.114476329</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -950,7 +950,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.141943604</v>
+        <v>0.067702974</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -958,7 +958,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>-0.128069699</v>
+        <v>-0.154675907</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -966,7 +966,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>-0.184321031</v>
+        <v>-0.140164361</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -974,7 +974,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>-0.295048147</v>
+        <v>-0.323887601</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -982,7 +982,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.000863509</v>
+        <v>0.04418762</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -990,7 +990,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.395999432</v>
+        <v>0.400949576</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -998,7 +998,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.049283478</v>
+        <v>0.071259618</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1006,7 +1006,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>-0.165615574</v>
+        <v>-0.189579175</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1014,7 +1014,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.082645178</v>
+        <v>0.06696640299999999</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1022,7 +1022,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>-0.008177904</v>
+        <v>-0.082723792</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1030,7 +1030,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>-0.10994596</v>
+        <v>0.011222476</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1038,7 +1038,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.11738544</v>
+        <v>0.112965522</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1046,7 +1046,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.180298641</v>
+        <v>0.159667841</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1054,7 +1054,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>-0.020335652</v>
+        <v>-0.009340342</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1062,7 +1062,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.027786965</v>
+        <v>0.010392343</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>-0.122492179</v>
+        <v>-0.106651159</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1078,7 +1078,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>-0.023993032</v>
+        <v>-0.011075524</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1086,7 +1086,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.221466526</v>
+        <v>0.194999854</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1094,7 +1094,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>-0.039410084</v>
+        <v>-0.06378718799999999</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1102,7 +1102,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>-0.057580084</v>
+        <v>-0.045034885</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1110,7 +1110,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.186976776</v>
+        <v>0.173100504</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1118,7 +1118,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>-0.029948983</v>
+        <v>-0.010282529</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1126,7 +1126,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.052329801</v>
+        <v>0.094190442</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1134,7 +1134,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.020575723</v>
+        <v>0.044694176</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1142,7 +1142,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.028963916</v>
+        <v>0.052367868</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1150,7 +1150,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>-0.037427075</v>
+        <v>-0.058467018</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1158,7 +1158,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0.038027383</v>
+        <v>0.067675821</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1166,7 +1166,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>-0.148514017</v>
+        <v>-0.113830893</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1174,7 +1174,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>-0.084329583</v>
+        <v>-0.030414354</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1182,7 +1182,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0.018245783</v>
+        <v>0.042017394</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1190,7 +1190,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>-0.07523677500000001</v>
+        <v>-0.06637910299999999</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1198,7 +1198,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>-0.060951054</v>
+        <v>-0.026684042</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1206,7 +1206,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0.073537007</v>
+        <v>0.119032121</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1214,7 +1214,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>-0.140593737</v>
+        <v>-0.117996948</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1222,7 +1222,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>0.101332061</v>
+        <v>0.138562426</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1230,7 +1230,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0.001327155</v>
+        <v>0.006768323</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1238,7 +1238,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>0.036141682</v>
+        <v>0.062455424</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1246,7 +1246,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>0.01256575</v>
+        <v>0.030197182</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1254,7 +1254,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>-0.030965047</v>
+        <v>-0.010535627</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1262,7 +1262,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>-0.07770210499999999</v>
+        <v>-0.067032019</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1270,7 +1270,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>-0.053317692</v>
+        <v>-0.06631896900000001</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1278,7 +1278,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0.132064983</v>
+        <v>0.120439429</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1286,7 +1286,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>-0.264641434</v>
+        <v>-0.206220964</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1294,7 +1294,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0.152247325</v>
+        <v>0.226510605</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1302,7 +1302,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>0.133808509</v>
+        <v>0.178263064</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1310,7 +1310,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>0.091882855</v>
+        <v>0.087851041</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1318,7 +1318,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>0.106028683</v>
+        <v>0.109401843</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1326,7 +1326,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>0.090502053</v>
+        <v>0.12891979</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1334,7 +1334,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>0.115060478</v>
+        <v>0.136094716</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1342,7 +1342,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>-0.009161973</v>
+        <v>-0.044693919</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1350,7 +1350,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>-0.07086888</v>
+        <v>-0.021595968</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1358,7 +1358,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>-0.237799063</v>
+        <v>-0.21338353</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1366,7 +1366,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>-0.016707871</v>
+        <v>0.015409064</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1374,7 +1374,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>0.076240145</v>
+        <v>0.08630738</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1382,7 +1382,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>-0.003606285</v>
+        <v>-0.031983804</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1390,7 +1390,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>0.15577212</v>
+        <v>0.08766318400000001</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1398,7 +1398,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>-0.009099459000000001</v>
+        <v>0.003020476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>